<commit_message>
frontend gallery dan article
gallery udah pasang, article sebagian terpasang
</commit_message>
<xml_diff>
--- a/datatable.xlsx
+++ b/datatable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="amd_meta" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="39">
   <si>
     <t>for</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>default: #</t>
+  </si>
+  <si>
+    <t>logo</t>
   </si>
 </sst>
 </file>
@@ -672,7 +675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -1064,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,14 +1080,15 @@
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1101,28 +1105,31 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1151,13 +1158,16 @@
         <v>19</v>
       </c>
       <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1174,10 +1184,10 @@
         <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
         <v>23</v>
@@ -1189,9 +1199,12 @@
         <v>23</v>
       </c>
       <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
         <v>25</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
kingdom finance rampung dan data dummy
kingdom finance rampung dan data dummy
</commit_message>
<xml_diff>
--- a/datatable.xlsx
+++ b/datatable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="amd_meta" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,16 @@
     <sheet name="amd_article" sheetId="7" r:id="rId8"/>
     <sheet name="amd_contact" sheetId="8" r:id="rId9"/>
     <sheet name="amd_users" sheetId="10" r:id="rId10"/>
+    <sheet name="amd_partner" sheetId="11" r:id="rId11"/>
+    <sheet name="amd_social" sheetId="12" r:id="rId12"/>
+    <sheet name="amd_website" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="56">
   <si>
     <t>for</t>
   </si>
@@ -163,9 +166,6 @@
     <t>access</t>
   </si>
   <si>
-    <t>0=spesific, 1=all</t>
-  </si>
-  <si>
     <t>if access = 0, nulable</t>
   </si>
   <si>
@@ -173,6 +173,27 @@
   </si>
   <si>
     <t>id_article_category</t>
+  </si>
+  <si>
+    <t>0=all, 1=all except edit or create user, 2=spe</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>google_map_url</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>brief</t>
   </si>
 </sst>
 </file>
@@ -623,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,10 +699,10 @@
         <v>44</v>
       </c>
       <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" t="s">
         <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -708,6 +729,273 @@
       </c>
       <c r="H3" t="s">
         <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1565,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection sqref="A1:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H1" sqref="H1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,12 +1731,12 @@
     <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -1463,36 +1751,39 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -1504,11 +1795,11 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
         <v>38</v>
       </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
       <c r="I2" t="s">
         <v>19</v>
       </c>
@@ -1522,13 +1813,16 @@
         <v>19</v>
       </c>
       <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
         <v>33</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1548,13 +1842,13 @@
         <v>23</v>
       </c>
       <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s">
         <v>23</v>
@@ -1566,9 +1860,12 @@
         <v>23</v>
       </c>
       <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
         <v>25</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>